<commit_message>
GUI is working, can merge csv files
</commit_message>
<xml_diff>
--- a/sample_output.xlsx
+++ b/sample_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Desktop\Projects\csv_to_pivotChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F511DA31-DA8F-46CB-8DE3-784692D24D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264756D9-07E8-4C23-83FD-327C24C70339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -2108,7 +2108,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
@@ -2344,7 +2344,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>